<commit_message>
Add 9 papers via GUI
</commit_message>
<xml_diff>
--- a/submit_template.xlsx
+++ b/submit_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20152" windowHeight="9855"/>
+    <workbookView windowWidth="22192" windowHeight="10455"/>
   </bookViews>
   <sheets>
     <sheet name="Papers" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="125">
   <si>
     <t>doi</t>
   </si>
@@ -84,6 +84,21 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>show in readme</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>submission time</t>
+  </si>
+  <si>
+    <t>conflict marker</t>
+  </si>
+  <si>
+    <t>invalid fields</t>
   </si>
   <si>
     <t>10.1609/icwsm.v19i1.35837</t>
@@ -146,6 +161,312 @@
   <si>
     <t>[引用句]Serving as a foundational critique within the transition from static classification to dynamic social simulation, Giorgi et al. (2025) demonstrate that although human perception of hate speech is fundamentally shaped by the interplay between annotator and target demographics, current persona-based LLMs fail to faithfully emulate these emergent sociological biases, highlighting a critical gap in the development of realistic AI agents.
 [翻译] 作为从静态分类向动态社会仿真过渡过程中的一项基础性批判研究，Giorgi等人（2025）证明，尽管人类对仇恨言论的感知从根本上受标注者与目标人口统计特征交互作用的影响，但当前的基于角色的LLM无法忠实地模拟这些涌现的社会学偏差，突显了构建逼真AI智能体方面的一个关键差距。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://doi.org/10.48550/arXiv.2402.18950</t>
+  </si>
+  <si>
+    <t>PopALM: Popularity-aligned language models for social media trendy response prediction</t>
+  </si>
+  <si>
+    <t>Erxin Yu1,Jing Li1∗,Chunpu Xu</t>
+  </si>
+  <si>
+    <t>2024-05</t>
+  </si>
+  <si>
+    <t>Social Content Generation</t>
+  </si>
+  <si>
+    <t>Motivated by the need to simulate mainstream public reactions on social media, this study identifies response popularity—quantified by "like" counts—as a crucial yet noisy signal for aligning language models with collective preferences.
+[翻译] 出于模拟社交媒体上主流公众反应的需求，本研究将通过“点赞数”量化的回复流行度视为一种关键信号，旨在将语言模型与群体偏好对齐，尽管该指标本身存在噪声。</t>
+  </si>
+  <si>
+    <t>The authors propose PopALM, which introduces a curriculum learning-enhanced Proximal Policy Optimization (CL-PPO) strategy to robustly align generation with popularity by mitigating the significant noise inherent in
+[翻译] 作者提出了 PopALM，该模型引入了一种增强了课程学习的近端策略优化（CL-PPO）策略，通过缓解原始互动指标中存在的显著噪声，稳健地将生成内容与流行度对齐。</t>
+  </si>
+  <si>
+    <t>The framework follows a sequential "SFT-RM-RL" pipeline, where the CL-PPO algorithm specifically incorporates reward enhancement, ranking, and self-paced sampling to transition training from high-confidence samples to complex scenarios, thereby filtering environmental noise.
+[翻译] 该框架遵循顺序的“有监督微调-奖励建模-强化学习”流程，其中CL-PPO算法特别结合了奖励增强、排序和自步采样机制，以实现从高置信度样本到复杂场景的过渡训练，从而过滤环境噪声。</t>
+  </si>
+  <si>
+    <t>Experiments on a large-scale Weibo benchmark demonstrate that PopALM outperforms state-of-the-art baselines in both automatic metrics and human evaluation, generating responses that are more specific and aligned with public sentiment.
+[翻译] 在大规模微博基准上的实验表明，PopALM 在自动指标和人工评估方面均优于最先进的基线模型，生成的回复更加具体且符合公众情绪。</t>
+  </si>
+  <si>
+    <t>A primary limitation lies in the reliance on "like" counts as the sole proxy for popularity, which may not fully capture multi-dimensional user engagement or generalize across different platform algorithms.
+[翻译] 一个主要的局限性在于依赖“点赞数”作为衡量流行度的单一代理指标，这可能无法完全捕捉多维度的用户参与度，也难以在不同平台的算法间泛化。</t>
+  </si>
+  <si>
+    <t>https://aclanthology.org/2024.lrec-main.1127/</t>
+  </si>
+  <si>
+    <t>https://github.com/ErxinYu/PopALM</t>
+  </si>
+  <si>
+    <t>LREC-COLING 2024</t>
+  </si>
+  <si>
+    <t>先练“选手”（SFT），再练“裁判”（RM），最后让“裁判”指导“选手”训练（RL）</t>
+  </si>
+  <si>
+    <t>PopALM.png</t>
+  </si>
+  <si>
+    <t>Social media platforms are daily exhibiting millions of events. To preliminarily predict the mainstream public reaction to these events, we study trendy response prediction to automatically generate top-liked user replies to social media events. While previous works focus on generating responses without factoring in popularity, we propose Popularity-Aligned Language Models (PopALM) to distinguish responses liked by a larger audience through reinforcement learning. Recognizing the noisy labels from user “likes”, we tailor-make curriculum learning in proximal policy optimization (PPO) to help models capture the essential samples for easy-to-hard training. In experiments, we build a large-scale Weibo dataset for trendy response prediction, and its results show that PopALM can help boost the performance of advanced language models.</t>
+  </si>
+  <si>
+    <t>[备注]该论文在会议上没有doi，使用的是arxiv版的doi【经典微调+RL范式】噪声指的是受各种因素影响，点赞数的具体值难以公平对比&lt;br&gt;[引用文]
+In the pursuit of simulating collective social behaviors rather than merely generating coherent text, aligning models with mainstream public sentiment becomes critical. However, social feedback signals, such as "like" counts, are often fraught with noise stemming from non-content factors like posting time or author influence. To address this, PopALM (Yu et al., 2024) proposes a PPO algorithm enhanced by curriculum learning. This approach operates on the premise that models should prioritize high-confidence samples—where popularity strongly correlates with content quality—to establish a robust foundation. By adopting a self-paced sampling strategy that transitions from easy-to-learn instances to noisier ones, PopALM effectively mitigates the significant noise inherent in using "like" counts as popularity indicators.
+[翻译]
+在追求模拟群体社会行为而非仅仅生成连贯文本的过程中，将模型与主流公众情绪对齐变得至关重要。然而，诸如“点赞数”之类的社会反馈信号往往充满了源自非内容因素（如发布时间或作者影响力）的噪声。针对这一问题，PopALM (Yu et al., 2024) 提出了一种增强了课程学习的PPO算法。该方法基于这样一个前提：模型应优先学习那些置信度高（即流行度与内容质量强相关）的样本，从而打下坚实的基础。通过采用一种从易学样本到噪声样本过渡的自步采样策略，PopALM 有效缓解了点赞数作为热度指标存在大量噪声的问题。</t>
+  </si>
+  <si>
+    <t>10.1609/icwsm.v19i1.35818</t>
+  </si>
+  <si>
+    <t>Identifying and Investigating Global News Coverage of Critical Events Such as Disasters and Terrorist Attacks</t>
+  </si>
+  <si>
+    <t>Erica Cai1,Xi Chen1,Reagan Grey Keeney1,Ethan Zuckerman1,Brendan O'Connor1,Przemyslaw A.Grabowicz</t>
+  </si>
+  <si>
+    <t>Event Extraction</t>
+  </si>
+  <si>
+    <t>Traditional computational studies of news coverage bias are hindered by the inability to efficiently and accurately identify articles discussing the same real-world event across massive, multilingual corpora without costly, language-specific training data.
+[翻译] 传统的新闻覆盖偏见计算研究面临一个瓶颈：难以在不依赖昂贵且语言特定的训练数据前提下，高效、精确地从大规模多语言语料库中识别出讨论同一现实事件的报道。</t>
+  </si>
+  <si>
+    <t>It introduces FAME, a scalable, zero-shot framework that utilizes minimalist “event fingerprints” (time, location, class) to match news articles across languages via a two-stage screening pipeline, eliminating the need for annotated training data.
+[翻译] 其提出了FAME框架，这是一个可扩展的零样本方法。它利用极简的“事件指纹”（时间、地点、类别），通过一个两级筛选流程实现跨语言新闻文章匹配，从而无需标注训练数据。</t>
+  </si>
+  <si>
+    <t>The method employs a two-stage pipeline: 1) Heuristic keyword filtering to recall candidate articles within a time window, followed by 2) a semantic filter using a large language model (LLM) for question-answering to achieve high-precision event-article matching.
+[翻译] 该方法采用一个两级处理流程：1）基于关键词的启发式过滤，用于在时间窗口内召回候选文章；2）利用大语言模型进行问答的语义过滤器，以实现高精度的事件-文章匹配。</t>
+  </si>
+  <si>
+    <t>FAME achieved state-of-the-art performance (average F1 &gt; 94% across English, Spanish, and French), and its application revealed that media attention to disasters and terrorist attacks is strongly correlated with death tolls, the GDP of the affected country, and bilateral trade volume.
+[翻译] FAME取得了先进的性能（在英、西、法语上平均F1&gt;94%）。应用该方法发现，媒体对灾害和恐怖袭击的关注度，与死亡人数、受影响国家的GDP以及双边贸易额高度相关。</t>
+  </si>
+  <si>
+    <t>The reliance on a two-stage screening pipeline depends on the quality of external event databases (e.g., GTD), and the minimalist fingerprint design, while enabling scalability, can lead to ambiguities for events with similar metadata.
+[翻译] 两级筛选流程依赖于外部事件数据库（如GTD）的质量，且极简的指纹设计虽然保证了可扩展性，但可能导致具有相似元数据的事件产生匹配歧义。</t>
+  </si>
+  <si>
+    <t>https://ojs.aaai.org/index.php/ICWSM/article/view/35818</t>
+  </si>
+  <si>
+    <t>https://github.com/social-info-lab/disaster_event_analysis</t>
+  </si>
+  <si>
+    <t>[AI generated] **中文标题：** 灾害与恐怖袭击等重大事件的全球新闻报道识别与调查分析
+**说明：** 该翻译准确传达了原标题的核心信息，即“识别”与“调查/分析”全球新闻报道。采用“重大事件”概括“Critical Events”，并使用“灾害与恐怖袭击”具体化其范畴，符合中文论文标题简洁、专业的学术风格。</t>
+  </si>
+  <si>
+    <t>两级匹配筛选要求新闻，关键词匹配初步筛选（关键词通过启发式方法获得）-&gt;事件抽取</t>
+  </si>
+  <si>
+    <t>figures/FAME.png;figures/FAME2.png</t>
+  </si>
+  <si>
+    <t>Comparative studies of news coverage are challenging to conduct because methods to identify news articles about the same event in different languages require expertise that is difficult to scale. We introduce an AI-powered method for identifying news articles based on an event fingerprint, which is a minimal set of metadata required to identify critical events. Our event coverage identification method, FINGERPRINT TO ARTICLE MATCHING FOR EVENTS (FAME), efficiently identifies news articles about critical world events, specifically terrorist attacks and several types of natural disasters. FAME does not require training data and is able to automatically and efficiently identify news articles that discuss an event given its fingerprint: time, location, and class (such as storm or flood). The method achieves state-of-the-art performance and scales to massive databases of tens of millions of news articles and hundreds of events happening globally. We use FAME to identify 27,441 articles that cover 470 natural disaster and terrorist attack events that happened in 2020. To this end, we use a massive database of news articles in three languages from MediaCloud, and three widely used, expert-curated databases of critical events: EM-DAT, USGS, and GTD. Our case study reveals patterns consistent with prior literature: coverage of disasters and terrorist attacks correlates to death counts, to the GDP of a country where the event occurs, and to trade volume between the reporting country and the country where the event occurred. We share our NLP annotations and cross-country media attention data to support the efforts of researchers and media monitoring organizations.</t>
+  </si>
+  <si>
+    <t>[引用文]Cai et al. (2025) propose the FAME framework, aiming to efficiently and accurately identify news reports on specific events from massive, multilingual news streams. Its innovation lies in a two-stage, zero-shot methodology. The framework first applies heuristic filtering using event “fingerprints” (time, location, category) to retrieve candidate articles, followed by a refinement step leveraging an LLM for precise event-article matching. This approach enables scalable, training-free analysis, successfully linking over 27,000 articles to 470 global events.
+[翻译]
+Cai等人(2025)提出的FAME框架，旨在从海量、多语言的新闻流中高效、精确地识别出关于特定事件的报道，其创新在于一种两级、零样本的方法。它首先使用事件“指纹”（时间、地点、类别）进行启发式过滤以获取候选文章，随后通过基于LLM进行事件匹配。这实现了可扩展的、免训练的分析，成功将超过2.7万篇文章与470个全球事件关联起来。</t>
+  </si>
+  <si>
+    <t>10.1609/aaai.v38i16.29730</t>
+  </si>
+  <si>
+    <t>Is a Large Language Model a Good Annotator for Event Extraction?</t>
+  </si>
+  <si>
+    <t>Ruirui Chen1,Chengwei Qin,Weifeng Jiang,Dongkyu Choi</t>
+  </si>
+  <si>
+    <t>2024-03-24</t>
+  </si>
+  <si>
+    <t>在提示中使用上下文示例来引导大语言模型生成与目标基准数据集分布和标注模式对齐的新样本，从而直接解决数据不平衡问题。</t>
+  </si>
+  <si>
+    <t>[AI generated] Employing LLMs as expert annotators with in-context examples to generate distribution-aligned data, directly addressing data scarcity and imbalance.
+[翻译]
+利用大语言模型作为专家标注器，结合上下文示例生成分布对齐的数据，直接解决数据稀缺与不平衡问题。</t>
+  </si>
+  <si>
+    <t>针对“训练样本稀少的（长尾）事件类型，使用合适的prompt模板（包含真实例子）要求LLM生成标注，进行质量筛选，合并到原始数据集，最终通过实验与合并前的效果比较</t>
+  </si>
+  <si>
+    <t>Fine-tuning models like BERT-CRF on the GPT-4-augmented ACE 2005 data led to consistent F1-score improvements in both Event Detection and Argument Extraction tasks, proving the high utility of LLM-generated annotations as a training resource.
+[翻译]
+在GPT-4增强的ACE 2005数据上微调BERT-CRF等模型，在事件检测和论元抽取任务中均带来了F1分数的持续提升，证明了LLM生成的标注作为训练资源的高效用。</t>
+  </si>
+  <si>
+    <t>高度依赖LLM自身能力</t>
+  </si>
+  <si>
+    <t>https://ojs.aaai.org/index.php/AAAI/article/view/29730</t>
+  </si>
+  <si>
+    <t>https://github.com/shiqinghuayi19/LLMforEvent</t>
+  </si>
+  <si>
+    <t>AAAI</t>
+  </si>
+  <si>
+    <t>[AI generated] **中文标题：大语言模型是事件抽取的优秀标注工具吗？**
+**翻译说明：**
+1.  **准确性**：标题直译核心问题，明确点明研究焦点——评估大语言模型在事件抽取任务中作为“标注工具”的潜力与效能。
+2.  **专业性**：采用“事件抽取”、“标注工具”等标准领域术语，符合自然语言处理领域的学术表达习惯。
+3.  **学术风格**：以疑问句式呈现</t>
+  </si>
+  <si>
+    <t>[AI generated] This method uses LLMs as expert annotators to generate high-quality training data, akin to employing a master chef to prepare ingredients for a specialized dish. [翻译]该方法利用大语言模型作为专家标注员生成高质量训练数据，如同聘请主厨为特色菜肴准备食材。</t>
+  </si>
+  <si>
+    <t>figures/Annotator for Event Extraction.png</t>
+  </si>
+  <si>
+    <t>Event extraction is an important task in natural language processing that focuses on mining event-related information from unstructured text. Despite considerable advancements, it is still challenging to achieve satisfactory performance in this task, and issues like data scarcity and imbalance obstruct progress. In this paper, we introduce an innovative approach where we employ Large Language Models (LLMs) as expert annotators for event extraction. We strategically include sample data from the training dataset in the prompt as a reference, ensuring alignment between the data distribution of LLM-generated samples and that of the benchmark dataset. This enables us to craft an augmented dataset that complements existing benchmarks, alleviating the challenges of data imbalance and scarcity and thereby enhancing the performance of fine-tuned models. We conducted extensive experiments to validate the efficacy of our proposed method, and we believe that this approach holds great potential for propelling the development and application of more advanced and reliable event extraction systems in real-world scenarios.</t>
+  </si>
+  <si>
+    <t>[引用文]To overcome data scarcity in specialized tasks within event extraction, large language models (LLMs) can be utilized as data augmentation tools. The work by Chen et al. (2024) exemplifies this by employing LLMs as structured annotators: using few-shot prompting with models such as GPT-4, they generate synthetic training data aligned with target schemas. This augmentation strategy effectively alleviates long-tail data imbalance and delivers measurable performance improvements for downstream extraction models.
+[翻译]
+为克服事件抽取领域专业任务中的数据稀缺问题，可以将大语言模型作为数据增强工具。Chen等人(2024)的研究通过将大语言模型用作结构化标注器来展示这一点：他们使用少量示例提示GPT-4等模型，生成与目标模式对齐的合成训练数据。这种增强策略有效缓解了长尾数据不平衡问题，为下游抽取模型带来了可观的性能提升。</t>
+  </si>
+  <si>
+    <t>10.1109/TPAMI.2022.3144993</t>
+  </si>
+  <si>
+    <t>Reinforced, Incremental and Cross-Lingual Event Detection From Social Messages</t>
+  </si>
+  <si>
+    <t>Hao Peng,Ruitong Zhang,Shaoning Li,Yuwei Cao,Shirui Pan,Philip S. Yu</t>
+  </si>
+  <si>
+    <t>2023-01-01</t>
+  </si>
+  <si>
+    <t>Event detection in social media streams is challenged by ambiguous event features, dispersed text content, multilingualism, and long-tail distribution, where traditional methods struggle in dynamic, incremental, and cross-lingual scenarios.
+[翻译]
+社交媒体流中的事件检测面临事件特征模糊、文本内容分散、多语言和长尾分布等挑战，传统方法在动态、增量和跨语言场景中表现不佳。</t>
+  </si>
+  <si>
+    <t>Its core advancement lies in enabling continuous, cross-lingual social event detection through a life-cycle mechanism that dynamically updates both the message graph and model without full retraining.
+[翻译]
+其核心进步在于，通过一个能动态更新消息图与模型而无需全量重训练的生命周期机制，实现了持续的、跨语言的社交事件检测。</t>
+  </si>
+  <si>
+    <t>The pipeline includes: (1) constructing a weighted multi-relational graph from social messages; (2) using multi-agent reinforcement learning to learn relation-specific thresholds for neighbor selection and aggregation; (3) training with balanced sampling-based contrastive learning; (4) clustering via DRL-optimized DBSCAN; and (5) enabling incremental updates and cross-lingual transfer via parameter preservation.
+[翻译]
+流程包括：(1) 从社交消息构建加权多关系图；(2) 使用多智能体强化学习学习关系特定的阈值以进行邻居选择和聚合；(3) 通过基于平衡采样的对比学习训练；(4) 使用DRL优化的DBSCAN聚类；(5) 通过参数保留支持增量更新和跨语言迁移。</t>
+  </si>
+  <si>
+    <t>On Twitter streams, FinEvent significantly outperforms baselines in offline, online, and cross-lingual detection tasks, with improvements of 14%-118% in NMI, 8%-170% in AMI, and 2%-21% in ARI, demonstrating robust performance across diverse settings.
+[翻译]
+在Twitter流数据上，FinEvent在离线、在线和跨语言检测任务中显著优于基线，NMI提升14%-118%，AMI提升8%-170%，ARI提升2%-21%，展现了在不同设置下的鲁棒性能。</t>
+  </si>
+  <si>
+    <t>Limitations include high computational complexity, dependence on external translation for low-resource languages, potential knowledge forgetting during incremental updates, and limited generalization due to evaluation primarily on Twitter data.
+[翻译]
+局限性包括计算复杂度高、对低资源语言依赖外部翻译、增量更新中可能遗忘早期知识，以及由于主要基于Twitter数据评估导致的泛化性有限。</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/9693189/</t>
+  </si>
+  <si>
+    <t>https://github.com/RingBDStack/FinEvent</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Pattern Analysis and Machine Intelligence</t>
+  </si>
+  <si>
+    <t>[AI generated] **中文标题：** 基于强化、增量与跨语言学习的社交媒体消息事件检测
+**说明：** 该翻译准确传达了原标题“Reinforced, Incremental and Cross-Lingual Event Detection From Social Messages”的核心要素：
+*   **“Reinforced”** 译为“强化”，对应论文中使用的强化学习方法。
+*   **“Incremental”** 译为“增量”，体现了模型对流式数据的持续学习能力。
+*   **“Cross</t>
+  </si>
+  <si>
+    <t>[AI generated] FinEvent is like a multilingual, self-optimizing news curator that continuously learns and adapts from live social media streams. [翻译] FinEvent 如同一个多语言的、自优化的新闻策展人，能从实时社交媒体流中持续学习与适应。</t>
+  </si>
+  <si>
+    <t>figures/FinEvent.png</t>
+  </si>
+  <si>
+    <t>Detecting hot social events (e.g., political scandal, momentous meetings, natural hazards, etc.) from social messages is crucial as it highlights significant happenings to help people understand the real world. On account of the streaming nature of social messages, incremental social event detection models in acquiring, preserving, and updating messages over time have attracted great attention. However, the challenge is that the existing event detection methods towards streaming social messages are generally confronted with ambiguous events features, dispersive text contents, and multiple languages, and hence result in low accuracy and generalization ability. In this paper, we present a novel reinForced, incremental and cross-lingual social Event detection architecture, namely FinEvent, from streaming social messages. Concretely, we first model social messages into heterogeneous graphs integrating both rich meta-semantics and diverse meta-relations, and convert them to weighted multi-relational message graphs. Second, we propose a new reinforced weighted multi-relational graph neural network framework by using a Multi-agent Reinforcement Learning algorithm to select optimal aggregation thresholds across different relations/edges to learn social message embeddings. To solve the long-tail problem in social event detection, a balanced sampling strategy guided Contrastive Learning mechanism is designed for incremental social message representation learning. Third, a new Deep Reinforcement Learning guided density-based spatial clustering model is designed to select the optimal minimum number of samples required to form a cluster and optimal minimum distance between two clusters in social event detection tasks. Finally, we implement incremental social message representation learning based on knowledge preservation on the graph neural network and achieve the transferring cross-lingual social event detection. We conduct extensive experiments to evaluate the FinEvent on Twitter streams, demonstrating a significant and consistent improvement in model quality with 14%–118%, 8%–170%, and 2%–21% increases in performance on offline, online, and cross-lingual social event detection tasks.</t>
+  </si>
+  <si>
+    <t>[引用文]Peng et al. (2023) proposed FinEvent, a reinforced, incremental, and cross-lingual detection architecture. Its core innovation lies in a life-cycle learning mechanism that supports incremental adaptation: the system dynamically updates a multi-relational message graph, employs multi-agent reinforcement learning to continuously optimize aggregation strategies, and utilizes a DRL-optimized clustering module to self-adjust parameters for each data block—enabling the model to co-evolve with the social data stream.
+[翻译]
+Peng等人（2023）提出了FinEvent，一个强化的增量与跨语言检测架构。其核心创新在于一个支持增量适应的生命周期学习机制：系统动态更新多关系消息图，并采用多智能体强化学习持续优化聚合策略，同时通过DRL优化的聚类模块实现每个数据块的自调参，使模型能随社交数据流共同演化。[notes]根据消息间的多种语义关系构建异构消息网络网络-&gt;通过多智能体强化学习得到每个关系的保留阈值（多智能体强化指的是每个智能体负责一个关系），对于每个消息节点的每个关系图，通过保留阈值剪除掉对聚合作用低的邻居节点-&gt;先图内聚合，再图间聚合得到每个节点的特征向量-&gt;使用Triplet Loss（拉近同类消息、推远异类消息）和Global-Local Loss（保持图结构的全局一致性）两个损失函数进行GNN训练，得到不同事件区分能力-&gt;使用DRL-DBSCAN进行自适应聚类，得到事件分类输出-&gt;支持增量更新与跨语言迁移</t>
+  </si>
+  <si>
+    <t>10.1609/aaai.v38i20.30252</t>
+  </si>
+  <si>
+    <t>Harnessing Network Effect for Fake News Mitigation: Selecting Debunkers via Self-Imitation Learning</t>
+  </si>
+  <si>
+    <t>Xiaofei Xu, Ke Deng, Michael Dann, Xiuzhen Zhang</t>
+  </si>
+  <si>
+    <t>Misinformation Analysis</t>
+  </si>
+  <si>
+    <t>Current approaches to multi-stage fake news mitigation often fail to address the episodic reward problem, where the effect of selecting an individual debunker cannot be measured until the campaign concludes. This sparse and delayed feedback limits the applicability of standard Reinforcement Learning (RL) in real-world social networks.
+[翻译]
+现有的多阶段假新闻治理方法往往未能解决片段式奖励问题，即选择单个辟谣者的效果只有在活动结束时才能衡量。这种稀疏且延迟的反馈限制了标准强化学习在现实社交网络中的适用性。</t>
+  </si>
+  <si>
+    <t>The authors propose NAGASIL, introducing two key enhancements to Self-Imitation Learning: 1) Negative Sampling, which leverages low-reward historical episodes to explicitly penalize poor debunker selections, and 2) State Augmentation, which enriches the observed state by integrating historical state-action sequences from the same campaign to address partial observability.
+[翻译]
+作者提出了NAGASIL，为自模仿学习引入了两个关键增强：1) 负采样，利用历史低奖励片段显式惩罚不良的辟谣者选择；2) 状态增强，通过融合同一活动中的历史状态-动作序列来丰富观测状态，以应对部分可观测性问题。</t>
+  </si>
+  <si>
+    <t>The debunker selection is formulated as a sequential decision-making problem under a budget constraint. A generative adversarial framework is employed, where a generator selects debunkers and a discriminator distinguishes between state-action pairs from high-reward historical episodes and those generated by the current policy. The generator is trained by integrating signals from the discriminator, an entropy regularizer for exploration, and a novel regularizer derived from a negative sampling model trained on low-reward episodes. This process yields an optimal generator capable of outputting an effective debunker selection policy.
+[翻译]
+辟谣者选择被建模为预算约束下的序列决策问题。采用生成对抗框架，其中生成器选择辟谣者，判别器区分来自高奖励历史片段的状态-动作对与当前策略生成的对。生成器的训练整合了来自判别器的信号、用于探索的熵正则项，以及一个从低奖励片段训练得到的负采样模型所衍生的新正则项。该过程最终产生一个能输出有效辟谣者选择策略的最优生成器。</t>
+  </si>
+  <si>
+    <t>Experiments conducted on both real-world (Facebook) and synthetic (Twitter) networks demonstrate that NAGASIL outperforms state-of-the-art fake news mitigation baselines and standard self-imitation learning methods across various budgets, stage lengths, and network densities.
+[翻译]
+在真实世界（Facebook）和合成（Twitter）网络上的实验表明，NAGASIL在各种预算、阶段长度和网络密度设置下，均优于先进的假新闻治理基线方法和标准自模仿学习方法。</t>
+  </si>
+  <si>
+    <t>The proposed method operates under the assumption that the veracity of news is pre-determined, necessitating integration with an external fake news detection system. Future research could explore adaptive propagation models and the dynamic nature of user behavior.
+[翻译]
+所提方法基于新闻真伪已知的假设运行，因此需要与外部假新闻检测系统结合。未来研究可探索自适应的传播模型和用户行为的动态特性。</t>
+  </si>
+  <si>
+    <t>https://ojs.aaai.org/index.php/AAAI/article/view/30252</t>
+  </si>
+  <si>
+    <t>https://github.com/xxfwin/NAGASIL</t>
+  </si>
+  <si>
+    <t>[AI generated] 中文标题：**利用网络效应抑制虚假新闻：基于自模仿学习的辟谣者选择策略**
+（说明：该翻译在保持学术严谨性的同时，通过“抑制虚假新闻”准确传达“mitigation”的主动干预含义；“辟谣者选择策略”清晰体现了“selecting debunkers”的研究核心；副标题结构符合中文论文标题常见格式。）</t>
+  </si>
+  <si>
+    <t>一个辟谣者选择策略（MDP风格）的生成器</t>
+  </si>
+  <si>
+    <t>figures/NAGASIL.png</t>
+  </si>
+  <si>
+    <t>This study aims to minimize the influence of fake news on social networks by deploying debunkers to propagate true news. This is framed as a reinforcement learning problem, where, at each stage, one user is selected to propagate true news. A challenging issue is episodic reward where the "net" effect of selecting individual debunkers cannot be discerned from the interleaving information propagation on social networks, and only the collective effect from mitigation efforts can be observed. Existing Self-Imitation Learning (SIL) methods have shown promise in learning from episodic rewards, but are ill-suited to the real-world application of fake news mitigation because of their poor sample efficiency. To learn a more effective debunker selection policy for fake news mitigation, this study proposes NAGASIL - Negative sampling and state Augmented Generative Adversarial Self-Imitation Learning, which consists of two improvements geared towards fake news mitigation: learning from negative samples, and an augmented state representation to capture the "real" environment state by integrating the current observed state with the previous state-action pairs from the same campaign. Experiments on two social networks show that NAGASIL yields superior performance to standard GASIL and state-of-the-art fake news mitigation models.</t>
+  </si>
+  <si>
+    <t>[引用文]The work by Xu et al. (2024) marks a pivotal transition from merely recognizing patterns of disinformation to actively intervening to curtail its spread. By harnessing network effects within a reinforcement learning framework enhanced by self-imitative adversarial learning, their NAGASIL model transcends static pattern recognition. It implements a dynamic, goal-oriented policy learning process that provides actionable guidance for debunker selection strategies.
+[翻译]
+Xu等人（2024）的研究标志着一个关键的转变：从仅仅识别虚假信息模式，转向主动干预以遏制其传播。通过在一个由自模仿对抗学习增强的强化学习框架内利用网络效应，他们的NAGASIL模型超越了静态模式识别。它实现了一个动态的、目标导向的策略学习过程，为辟谣者选择策略提供了可行的指导。&lt;br&gt;[notes]1.这是一个对抗性学习框架，判别器希望好序列的置信度高，其他序列的置信度低，通过损失函数训练优化。生成器依据目标函数进行训练优化，目标函数包含三部分：判别器传来的对抗信号（置信度）、鼓励多样性的熵正则、负采样正则项（来自坏序列的距离（训练另一个模型以输出该值））。好经验和坏经验每轮通过奖励值V(τ) = -log(感染用户比例)获得。
+2.每**轮**中每个**阶段**选择一个用户恢复并作为辟谣者，预算减去其成本，进行w个**时间步**的辟谣。每个阶段的预算用完后，进行每轮一次的梯度更新和好坏序列评选，然后进入下一轮</t>
   </si>
 </sst>
 </file>
@@ -808,16 +1129,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1164,22 +1487,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="5" width="15" customWidth="1"/>
-    <col min="6" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="10" width="21" customWidth="1"/>
-    <col min="11" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="19" width="15" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="3" width="50" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="15" width="50" customWidth="1"/>
+    <col min="16" max="16" width="45" customWidth="1"/>
+    <col min="17" max="17" width="50" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="50" customWidth="1"/>
+    <col min="20" max="20" width="17" customWidth="1"/>
+    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="22" max="23" width="18" customWidth="1"/>
+    <col min="24" max="24" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1240,82 +1568,452 @@
       <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:24">
+    <row r="2" spans="1:24">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="S2" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="T2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:24">
+      <c r="A3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="T4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="T5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="T6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="T7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" display="https://aclanthology.org/2024.lrec-main.1127/"/>
+    <hyperlink ref="L3" r:id="rId2" display="https://github.com/ErxinYu/PopALM"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>